<commit_message>
Revised list of indicators 10-4-16
</commit_message>
<xml_diff>
--- a/Indicators/Indicators_Revised Descriptions.xlsx
+++ b/Indicators/Indicators_Revised Descriptions.xlsx
@@ -404,9 +404,6 @@
     <t>Yearly average mass (kg) of organisms per unit area.</t>
   </si>
   <si>
-    <t>Yearly verage number of species per unit area.</t>
-  </si>
-  <si>
     <t>Has the availability of alternative economic opportunities increased, decreased, or stayed the same after implementation of the reserve?</t>
   </si>
   <si>
@@ -435,6 +432,9 @@
   </si>
   <si>
     <t>Degree of knowledge the fishers have about the reserve type and reserve objectives.</t>
+  </si>
+  <si>
+    <t>Yearly average number of species per unit area.</t>
   </si>
 </sst>
 </file>
@@ -482,12 +482,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -502,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -534,6 +540,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,7 +830,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -854,11 +866,11 @@
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>6</v>
@@ -869,7 +881,7 @@
     </row>
     <row r="3" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -884,7 +896,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -899,7 +911,7 @@
     </row>
     <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -935,7 +947,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -949,7 +961,7 @@
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -964,7 +976,7 @@
     </row>
     <row r="9" spans="1:6" ht="143" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="12" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -986,7 +998,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>40</v>
@@ -994,11 +1006,11 @@
     </row>
     <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
-        <v>68</v>
+      <c r="B11" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>40</v>
@@ -1007,10 +1019,10 @@
     <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>70</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>40</v>
@@ -1023,11 +1035,11 @@
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>13</v>
@@ -1035,11 +1047,11 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>6</v>
@@ -1047,7 +1059,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1059,7 +1071,7 @@
     </row>
     <row r="16" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1071,11 +1083,11 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>40</v>
@@ -1083,7 +1095,7 @@
     </row>
     <row r="18" spans="1:5" s="10" customFormat="1" ht="39" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="12" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1095,7 +1107,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1107,11 +1119,11 @@
     </row>
     <row r="20" spans="1:5" s="10" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>6</v>
@@ -1119,7 +1131,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1131,7 +1143,7 @@
     </row>
     <row r="22" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="12" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -1146,7 +1158,7 @@
     </row>
     <row r="23" spans="1:5" ht="39" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1157,11 +1169,11 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Commiting files, hope this doesnt brake it
</commit_message>
<xml_diff>
--- a/Indicators/Indicators_Revised Descriptions.xlsx
+++ b/Indicators/Indicators_Revised Descriptions.xlsx
@@ -404,9 +404,6 @@
     <t>Yearly average mass (kg) of organisms per unit area.</t>
   </si>
   <si>
-    <t>Yearly verage number of species per unit area.</t>
-  </si>
-  <si>
     <t>Has the availability of alternative economic opportunities increased, decreased, or stayed the same after implementation of the reserve?</t>
   </si>
   <si>
@@ -435,6 +432,9 @@
   </si>
   <si>
     <t>Degree of knowledge the fishers have about the reserve type and reserve objectives.</t>
+  </si>
+  <si>
+    <t>Yearly average number of species per unit area.</t>
   </si>
 </sst>
 </file>
@@ -482,12 +482,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -502,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -534,6 +540,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,7 +830,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -854,11 +866,11 @@
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>6</v>
@@ -869,7 +881,7 @@
     </row>
     <row r="3" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -884,7 +896,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -899,7 +911,7 @@
     </row>
     <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -935,7 +947,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -949,7 +961,7 @@
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -964,7 +976,7 @@
     </row>
     <row r="9" spans="1:6" ht="143" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="12" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -986,7 +998,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>40</v>
@@ -994,11 +1006,11 @@
     </row>
     <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
-        <v>68</v>
+      <c r="B11" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>40</v>
@@ -1007,10 +1019,10 @@
     <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>70</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>40</v>
@@ -1023,11 +1035,11 @@
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>13</v>
@@ -1035,11 +1047,11 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>6</v>
@@ -1047,7 +1059,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1059,7 +1071,7 @@
     </row>
     <row r="16" spans="1:6" ht="39" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1071,11 +1083,11 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>40</v>
@@ -1083,7 +1095,7 @@
     </row>
     <row r="18" spans="1:5" s="10" customFormat="1" ht="39" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="12" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1095,7 +1107,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1107,11 +1119,11 @@
     </row>
     <row r="20" spans="1:5" s="10" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>6</v>
@@ -1119,7 +1131,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1131,7 +1143,7 @@
     </row>
     <row r="22" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="12" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -1146,7 +1158,7 @@
     </row>
     <row r="23" spans="1:5" ht="39" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1157,11 +1169,11 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Changed the descrtiption fort type of enforcement
</commit_message>
<xml_diff>
--- a/Indicators/Indicators_Revised Descriptions.xlsx
+++ b/Indicators/Indicators_Revised Descriptions.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jael Martinez\Documents\GitHub\Docs\Indicators\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +24,7 @@
     <author>JC</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -145,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0">
+    <comment ref="C9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0">
+    <comment ref="A13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
   <si>
     <t>Type of indicator</t>
   </si>
@@ -435,16 +430,13 @@
   </si>
   <si>
     <t>Degree of knowledge the fishers have about the reserve type and reserve objectives. Creation of a Knowledge index with 5 indicators (Type of reserve, Year of implementation, Density, Species richness, Predators abundance) where less than 3 right answers is a low knowledge of the reality, from 3 and 4 is intermediate knowledge and 5 is high.</t>
-  </si>
-  <si>
-    <t>Categorical / Descriptive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,30 +857,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +900,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -925,7 +917,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="25.5">
       <c r="A3" s="3"/>
       <c r="B3" s="12" t="s">
         <v>56</v>
@@ -940,7 +932,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="3"/>
       <c r="B4" s="12" t="s">
         <v>7</v>
@@ -955,7 +947,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="3"/>
       <c r="B5" s="12" t="s">
         <v>8</v>
@@ -973,7 +965,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="25.5">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
         <v>32</v>
@@ -991,7 +983,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="3"/>
       <c r="B7" s="12" t="s">
         <v>27</v>
@@ -1003,7 +995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1020,7 +1012,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="127.5">
       <c r="A9" s="3"/>
       <c r="B9" s="12" t="s">
         <v>49</v>
@@ -1038,7 +1030,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="25.5">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
         <v>12</v>
@@ -1050,7 +1042,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="63.75">
       <c r="A11" s="3"/>
       <c r="B11" s="12" t="s">
         <v>67</v>
@@ -1062,7 +1054,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="17" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="17" customFormat="1" ht="25.5">
       <c r="A12" s="14"/>
       <c r="B12" s="15" t="s">
         <v>68</v>
@@ -1077,7 +1069,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="25.5">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1091,7 +1083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" s="3"/>
       <c r="B14" s="12" t="s">
         <v>17</v>
@@ -1103,7 +1095,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="3"/>
       <c r="B15" s="12" t="s">
         <v>18</v>
@@ -1115,7 +1107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="25.5">
       <c r="A16" s="3"/>
       <c r="B16" s="12" t="s">
         <v>41</v>
@@ -1127,7 +1119,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="3"/>
       <c r="B17" s="12" t="s">
         <v>21</v>
@@ -1139,7 +1131,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="10" customFormat="1" ht="38.25">
       <c r="A18" s="9"/>
       <c r="B18" s="12" t="s">
         <v>43</v>
@@ -1151,7 +1143,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="3"/>
       <c r="B19" s="12" t="s">
         <v>22</v>
@@ -1160,10 +1152,10 @@
         <v>44</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="10" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="10" customFormat="1" ht="25.5">
       <c r="A20" s="9"/>
       <c r="B20" s="12" t="s">
         <v>45</v>
@@ -1175,7 +1167,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="3"/>
       <c r="B21" s="12" t="s">
         <v>23</v>
@@ -1187,7 +1179,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="25.5">
       <c r="A22" s="3"/>
       <c r="B22" s="12" t="s">
         <v>53</v>
@@ -1202,7 +1194,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="38.25">
       <c r="A23" s="3"/>
       <c r="B23" s="12" t="s">
         <v>52</v>
@@ -1214,7 +1206,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="25.5">
       <c r="B24" s="13" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
added changes during gp meeting
</commit_message>
<xml_diff>
--- a/Indicators/Indicators_Revised Descriptions.xlsx
+++ b/Indicators/Indicators_Revised Descriptions.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jael Martinez\Documents\GitHub\Docs\Indicators\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +29,7 @@
     <author>JC</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -95,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0">
+    <comment ref="E8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0">
+    <comment ref="C9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -164,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0">
+    <comment ref="A13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
   <si>
     <t>Type of indicator</t>
   </si>
@@ -342,9 +347,6 @@
     <t>Reserve type</t>
   </si>
   <si>
-    <t>Type of reserve (core zone, refugio pesquero, voluntarily owned), duration of reserve (temporary or permanent), and level of protection (partial, total).</t>
-  </si>
-  <si>
     <t>Management plan</t>
   </si>
   <si>
@@ -430,13 +432,25 @@
   </si>
   <si>
     <t>Degree of knowledge the fishers have about the reserve type and reserve objectives. Creation of a Knowledge index with 5 indicators (Type of reserve, Year of implementation, Density, Species richness, Predators abundance) where less than 3 right answers is a low knowledge of the reality, from 3 and 4 is intermediate knowledge and 5 is high.</t>
+  </si>
+  <si>
+    <t>Internal Regulation</t>
+  </si>
+  <si>
+    <t>Does the reserve has its own regulations?</t>
+  </si>
+  <si>
+    <t>Type of reserve (core zone, refugio pesquero, voluntarily owned), duration of reserve (temporary or permanent), and level of protection (partial, total). If it is inside or outside a TURF</t>
+  </si>
+  <si>
+    <t>Perceived Effectiveness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -857,30 +871,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -900,7 +914,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -908,7 +922,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>6</v>
@@ -917,13 +931,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5">
+    <row r="3" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>9</v>
@@ -932,13 +946,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>9</v>
@@ -947,13 +961,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
@@ -965,7 +979,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="25.5">
+    <row r="6" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="5" t="s">
         <v>32</v>
@@ -983,19 +997,19 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1003,7 +1017,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>9</v>
@@ -1012,13 +1026,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="127.5">
+    <row r="9" spans="1:6" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>9</v>
@@ -1030,37 +1044,37 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="25.5">
+    <row r="10" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63.75">
+    <row r="11" spans="1:6" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="B11" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="17" customFormat="1" ht="25.5">
+    <row r="12" spans="1:6" s="17" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>68</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>69</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>40</v>
@@ -1069,7 +1083,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="25.5">
+    <row r="13" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1077,25 +1091,25 @@
         <v>15</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="12" t="s">
         <v>18</v>
@@ -1107,114 +1121,133 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="25.5">
+    <row r="16" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="10" customFormat="1" ht="38.25">
+    <row r="18" spans="1:5" s="10" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="10" customFormat="1" ht="25.5">
+    <row r="20" spans="1:5" s="10" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="25.5">
+    <row r="22" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="38.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="25.5">
+    <row r="24" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>